<commit_message>
Made move combinations function
</commit_message>
<xml_diff>
--- a/Pokemon Go General Stats.xlsx
+++ b/Pokemon Go General Stats.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Important Personal\Tech Portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger\Documents\GitHub\Pokemon-GO-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48259190-3292-47A3-B712-4E9292D42D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4490B87-DB6A-4288-96E4-980B888A23F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D568CBEC-42C9-4DFF-B77D-963AE0693B08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{D568CBEC-42C9-4DFF-B77D-963AE0693B08}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="2" r:id="rId1"/>
     <sheet name="TypeChart" sheetId="4" r:id="rId2"/>
+    <sheet name="CP Multiplier" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="755">
   <si>
     <t>#</t>
   </si>
@@ -2292,13 +2293,19 @@
   </si>
   <si>
     <t>Attack</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>CP Multiplier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2306,16 +2313,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0571C2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF585858"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2323,12 +2356,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFB8D4DA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFB8D4DA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFB8D4DA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFB8D4DA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19252,8 +19309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9835875-88AD-4E04-BBEE-82806B8FB044}">
   <dimension ref="A1:D325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q29:R30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19470,7 +19527,8 @@
         <v>748</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -20156,7 +20214,8 @@
         <v>748</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -20982,7 +21041,8 @@
         <v>748</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -21276,7 +21336,8 @@
         <v>748</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -21430,7 +21491,8 @@
         <v>748</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -22018,7 +22080,8 @@
         <v>748</v>
       </c>
       <c r="D197">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -22564,7 +22627,8 @@
         <v>748</v>
       </c>
       <c r="D236">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -23054,7 +23118,8 @@
         <v>748</v>
       </c>
       <c r="D271">
-        <v>0</v>
+        <f>0.625^2</f>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -23811,6 +23876,841 @@
       </c>
       <c r="D325">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CBCDCF-5965-452E-B677-157CF99FBBE8}">
+  <dimension ref="A1:B102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.13513743180000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.16639787</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.192650919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.21573247000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.23657266129999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.25572004999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.27353038120000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.29024988000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.30605737750000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.32108759999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.33544503619999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.34921268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.3624577511</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.3752356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.387592416</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.39956728000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.41119355140000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.42249999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.43292640910000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.44310755000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.45305995910000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.4627984</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.47233609300000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.48168495</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.49085580029999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.49985844000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.50870176499999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>15</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.51739394999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.52594251130000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.53435429999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.54263573750000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>17</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.55079270000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>17.5</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.55883058620000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.56675450000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.57456913330000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>19</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.58227890000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>19.5</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.58988790719999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.59740000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.60482366509999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>21</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.61215730000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.61940412160000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>22</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.62656710000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.63364914319999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>23</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.64065295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.64758096659999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>24</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.65443563000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.66121925240000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>25</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.66793400000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.67458189589999995</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>26</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.68116489999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>26.5</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0.68768490380000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>27</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.69414365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.70054287000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>28</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.70688419999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>28.5</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.71316910909999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>29</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.71939909999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>29.5</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.7255756136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>30</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.73170000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>30.5</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0.73474100929999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>31</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.73776949999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.74078559379999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>32</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.74378942999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.74678121090000005</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>33</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.74976103999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.75272908670000005</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>34</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.75568550000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.75863036829999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>35</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.76156383999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>35.5</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.76448606470000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>36</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.76739716999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>36.5</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.7702972656</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>37</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.7731865</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.77606496160000005</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>38</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.77893274999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.78179005479999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>39</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.78463700000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.78747360749999995</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>40</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.7903</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.79280396799999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>41</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.79530000999999995</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>41.5</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.79780001499999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>42</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.80030000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>42.5</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.80279999499999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <v>43</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.80530000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>43.5</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.80779999999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>44</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.81029998999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>44.5</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.81279998499999995</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>45</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.81529998999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <v>45.5</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.81779999000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>46</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.82029998999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.82279999000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>47</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.82529998999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>47.5</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.82779999000000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>48</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.83029998999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>48.5</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.83279999000000005</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>49</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.83529998999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>49.5</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.83779999000000005</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>50</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.84029999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.84279999000000005</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>51</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0.84529999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>